<commit_message>
Penyesuaian dengan Input Baru
</commit_message>
<xml_diff>
--- a/data/DK_133_TF_Semester3_2025.xlsx
+++ b/data/DK_133_TF_Semester3_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Algoritma Genetika\scheduling-genetic-algorithm\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8ECD0BB-2D90-4AB2-8746-47D3BBC40A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11355F61-6707-4718-AEDE-534D81963C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="3110" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="77">
   <si>
     <t>NO</t>
   </si>
@@ -232,7 +232,52 @@
     <t>Tingkat</t>
   </si>
   <si>
-    <t>AB</t>
+    <t>HK, MI</t>
+  </si>
+  <si>
+    <t>GS, AN</t>
+  </si>
+  <si>
+    <t>EE, AS</t>
+  </si>
+  <si>
+    <t>MI, RM</t>
+  </si>
+  <si>
+    <t>NG, FF</t>
+  </si>
+  <si>
+    <t>MH, IP</t>
+  </si>
+  <si>
+    <t>RR, AR</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>NG</t>
+  </si>
+  <si>
+    <t>NP</t>
+  </si>
+  <si>
+    <t>SP, MI</t>
+  </si>
+  <si>
+    <t>DA, EB</t>
+  </si>
+  <si>
+    <t>MI, NP</t>
+  </si>
+  <si>
+    <t>NP, MI</t>
+  </si>
+  <si>
+    <t>MI, EB</t>
+  </si>
+  <si>
+    <t>EB, MI</t>
   </si>
 </sst>
 </file>
@@ -657,15 +702,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K16" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4.1796875" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="4" width="21.81640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="21.81640625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" style="11" customWidth="1"/>
     <col min="5" max="5" width="12.08984375" style="16" customWidth="1"/>
     <col min="6" max="6" width="7.90625" style="16" customWidth="1"/>
     <col min="7" max="7" width="4.453125" style="16" customWidth="1"/>
@@ -862,7 +908,7 @@
         <v>28</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M3" s="6">
         <v>0</v>
@@ -936,7 +982,7 @@
         <v>31</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M4" s="6">
         <v>0</v>
@@ -1010,7 +1056,7 @@
         <v>32</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M5" s="6">
         <v>0</v>
@@ -1084,7 +1130,7 @@
         <v>35</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="M6" s="6">
         <v>0</v>
@@ -1158,7 +1204,7 @@
         <v>37</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="M7" s="6">
         <v>0</v>
@@ -1232,7 +1278,7 @@
         <v>40</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="M8" s="6">
         <v>0</v>
@@ -1306,7 +1352,7 @@
         <v>41</v>
       </c>
       <c r="L9" s="17" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="M9" s="6">
         <v>0</v>
@@ -1380,7 +1426,7 @@
         <v>43</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="M10" s="6">
         <v>0</v>
@@ -1454,7 +1500,7 @@
         <v>45</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="M11" s="6">
         <v>0</v>
@@ -1528,7 +1574,7 @@
         <v>48</v>
       </c>
       <c r="L12" s="17" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="M12" s="6">
         <v>9121</v>
@@ -1602,7 +1648,7 @@
         <v>51</v>
       </c>
       <c r="L13" s="17" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="M13" s="6">
         <v>9121</v>
@@ -1676,7 +1722,7 @@
         <v>54</v>
       </c>
       <c r="L14" s="17" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="M14" s="6">
         <v>0</v>
@@ -1748,7 +1794,7 @@
         <v>55</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="M15" s="6">
         <v>0</v>
@@ -1820,7 +1866,7 @@
         <v>58</v>
       </c>
       <c r="L16" s="17" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="M16" s="6">
         <v>0</v>
@@ -1892,7 +1938,7 @@
         <v>59</v>
       </c>
       <c r="L17" s="17" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="M17" s="6">
         <v>0</v>

</xml_diff>